<commit_message>
modify data format, replace data in 2 diff dfs.
</commit_message>
<xml_diff>
--- a/data/data_fmt_readme.xlsx
+++ b/data/data_fmt_readme.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\webscrapy\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\factors_affecting_stock_price\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D87CD8-567F-4F05-8BCB-6E9D8994CBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3683DE9B-E0AD-4F0E-9234-2260A6543217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="1275" windowWidth="20025" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30120" yWindow="2715" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="항목설명" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="206">
   <si>
     <t>나스닥지수</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,18 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10년만기국채수익률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2년만기국채수익률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3개월만기국채수익률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>나스닥선물지수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -340,18 +328,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10_YEAR_BOND_YIELD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2_YEAR_BOND_YIELD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3_MONTH_BOND_YIELD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VIX</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -597,18 +573,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10_bond</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2_bond</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3_m_bond</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>vix</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -823,6 +787,58 @@
   </si>
   <si>
     <t>PrivateEquity_Purchase_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_usa_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_usa_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_usa_3m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_kor_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_kor_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10_YEAR_BOND_YIELD_korea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_YEAR_BOND_YIELD_korea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10_YEAR_BOND_YIELD_usa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_YEAR_BOND_YIELD_usa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3_MONTH_BOND_YIELD_usa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미국10년만기국채수익률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미국2년만기국채수익률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미국3개월만기국채수익률</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1148,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80437AA-7DDE-482B-8494-793A82C56F06}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1183,22 +1199,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1206,13 +1222,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1220,16 +1236,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1237,19 +1253,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1257,13 +1273,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1271,13 +1287,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1285,10 +1301,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
@@ -1299,13 +1315,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1313,13 +1329,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1327,13 +1343,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1341,10 +1357,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
@@ -1355,13 +1371,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1369,13 +1385,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1383,13 +1399,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1397,10 +1413,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
@@ -1411,13 +1427,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1425,10 +1441,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -1439,13 +1455,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1453,10 +1469,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -1467,13 +1483,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1481,10 +1497,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -1495,13 +1511,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>200</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1509,13 +1525,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>201</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1523,13 +1539,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1537,13 +1553,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>198</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1551,13 +1567,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1565,13 +1581,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1579,13 +1595,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1593,13 +1609,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1607,16 +1623,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1624,16 +1637,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>197</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" t="s">
-        <v>195</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1641,13 +1651,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="E32" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1655,13 +1668,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1669,10 +1685,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="C34" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
         <v>24</v>
@@ -1683,13 +1699,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1697,13 +1713,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1711,13 +1727,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="C37" t="s">
-        <v>199</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1725,13 +1741,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1739,13 +1755,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1753,13 +1769,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>200</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1767,13 +1783,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C41" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1781,13 +1797,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1795,13 +1811,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C43" t="s">
-        <v>201</v>
+        <v>90</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1809,13 +1825,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1823,13 +1839,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1837,16 +1853,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" t="s">
-        <v>192</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1854,13 +1867,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1868,13 +1881,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="E48" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1882,13 +1898,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C49" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1896,13 +1912,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1910,16 +1926,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D51" t="s">
-        <v>52</v>
-      </c>
-      <c r="E51" t="s">
-        <v>176</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1927,16 +1940,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D52" t="s">
-        <v>107</v>
-      </c>
-      <c r="E52" t="s">
-        <v>176</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1944,13 +1954,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C53" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D53" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="E53" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1958,13 +1971,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C54" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D54" t="s">
-        <v>53</v>
+        <v>101</v>
+      </c>
+      <c r="E54" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1972,13 +1988,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C55" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D55" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1986,16 +2002,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C56" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D56" t="s">
-        <v>69</v>
-      </c>
-      <c r="E56" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -2003,16 +2016,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D57" t="s">
-        <v>70</v>
-      </c>
-      <c r="E57" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -2020,13 +2030,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D58" t="s">
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="E58" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -2034,13 +2047,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D59" t="s">
-        <v>38</v>
+        <v>67</v>
+      </c>
+      <c r="E59" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -2048,13 +2064,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C60" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D60" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -2062,13 +2078,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C61" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D61" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -2076,13 +2092,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C62" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D62" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -2090,13 +2106,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C63" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D63" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -2104,13 +2120,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C64" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D64" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2118,13 +2134,41 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D65" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>178</v>
+      </c>
+      <c r="C66" t="s">
+        <v>110</v>
+      </c>
+      <c r="D66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>179</v>
+      </c>
+      <c r="C67" t="s">
+        <v>111</v>
+      </c>
+      <c r="D67" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
df.update, data folder arrange
</commit_message>
<xml_diff>
--- a/data/data_fmt_readme.xlsx
+++ b/data/data_fmt_readme.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\factors_affecting_stock_price\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ipynb\factors_affecting_stock_price\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3683DE9B-E0AD-4F0E-9234-2260A6543217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30120" yWindow="2715" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30120" yWindow="2715" windowWidth="20025" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="항목설명" sheetId="2" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="219">
   <si>
     <t>나스닥지수</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -533,320 +532,372 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>spx_f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spx_f_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kospi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kospi_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kosdaq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kosdaq_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dxy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>krw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vix_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_g_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sox</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pp_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fp_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itp_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>penp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>penp_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pep_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pp_con_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fp_con_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itp_con_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>penp_con_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pep_con_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gold_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rc1_pcr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rc2_pcr</t>
+  </si>
+  <si>
+    <t>rc3_pcr</t>
+  </si>
+  <si>
+    <t>rc4_pcr</t>
+  </si>
+  <si>
+    <t>fed_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fed_rate_ann</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fed_rate-imp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bok_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기준일 대비 -일로 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bok_rate_ann</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bok_rate-imp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fu_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>high</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>high_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>low</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>low_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vol_cr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거래일자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전일 지수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전일 변동률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1주 변동률 추이 검토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추후 검토(시계열분석 대체효과)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지난 5일간 순매수(+), 혹은 순매도(-)가 지속된 일수(+,-일수)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전전일대비 전일 변동률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Personal_Purchase_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foreigner_Purchase_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InvestmentTrust_Purchase_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pension_Purchase_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PrivateEquity_Purchase_number_of_consecutive_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_usa_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_usa_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_usa_3m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_kor_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bond_kor_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10_YEAR_BOND_YIELD_korea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_YEAR_BOND_YIELD_korea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10_YEAR_BOND_YIELD_usa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_YEAR_BOND_YIELD_usa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3_MONTH_BOND_YIELD_usa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미국10년만기국채수익률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미국2년만기국채수익률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미국3개월만기국채수익률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>spx_cr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>spx_f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spx_f_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kospi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kospi_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kosdaq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kosdaq_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wti</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dxy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>krw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vix_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_g_index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pp_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fp_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>itp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>itp_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>penp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>penp_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pep</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pep_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pp_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fp_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>itp_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>penp_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pep_con_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gold</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gold_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rc1_pcr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rc2_pcr</t>
-  </si>
-  <si>
-    <t>rc3_pcr</t>
-  </si>
-  <si>
-    <t>rc4_pcr</t>
-  </si>
-  <si>
-    <t>fed_rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fed_rate_ann</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fed_rate-imp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bok_rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기준일 대비 -일로 표시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bok_rate_ann</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bok_rate-imp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fu_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>op_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>open</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>high</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>high_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>low</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>low_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>close</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vol</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vol_cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>거래일자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전일 지수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전일 변동률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1주 변동률 추이 검토</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추후 검토(시계열분석 대체효과)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지난 5일간 순매수(+), 혹은 순매도(-)가 지속된 일수(+,-일수)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전전일대비 전일 변동률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Personal_Purchase_number_of_consecutive_days</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Foreigner_Purchase_number_of_consecutive_days</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvestmentTrust_Purchase_number_of_consecutive_days</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pension_Purchase_number_of_consecutive_days</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PrivateEquity_Purchase_number_of_consecutive_days</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bond_usa_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bond_usa_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bond_usa_3m</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bond_kor_10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bond_kor_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10_YEAR_BOND_YIELD_korea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2_YEAR_BOND_YIELD_korea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10_YEAR_BOND_YIELD_usa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2_YEAR_BOND_YIELD_usa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3_MONTH_BOND_YIELD_usa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국10년만기국채수익률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국2년만기국채수익률</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미국3개월만기국채수익률</t>
+    <t>spx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sox_cr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOX_INDEX_change_rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>필라델피아 반도체지수 변동률</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpi_anticipated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpi_previous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소비자물가지수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consumer Price Index</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예측 소비자물가지수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anticipated consumer price index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>previous consumer price index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이전 소비자물가지수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -858,6 +909,13 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -882,8 +940,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1163,11 +1224,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80437AA-7DDE-482B-8494-793A82C56F06}">
-  <dimension ref="A1:F67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1211,10 +1272,10 @@
         <v>119</v>
       </c>
       <c r="E1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1228,7 +1289,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1245,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1262,10 +1323,10 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" t="s">
         <v>183</v>
-      </c>
-      <c r="F4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1357,7 +1418,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>206</v>
       </c>
       <c r="C11" t="s">
         <v>62</v>
@@ -1371,7 +1432,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>205</v>
       </c>
       <c r="C12" t="s">
         <v>63</v>
@@ -1385,7 +1446,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C13" t="s">
         <v>64</v>
@@ -1399,7 +1460,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
         <v>65</v>
@@ -1413,7 +1474,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
         <v>68</v>
@@ -1427,7 +1488,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" t="s">
         <v>69</v>
@@ -1436,12 +1497,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
         <v>70</v>
@@ -1450,12 +1511,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
         <v>71</v>
@@ -1464,12 +1525,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
         <v>73</v>
@@ -1478,12 +1539,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
         <v>74</v>
@@ -1492,12 +1553,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
         <v>75</v>
@@ -1506,82 +1567,82 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D23" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D25" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D26" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s">
         <v>76</v>
@@ -1590,12 +1651,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C28" t="s">
         <v>78</v>
@@ -1604,12 +1665,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C29" t="s">
         <v>79</v>
@@ -1618,12 +1679,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C30" t="s">
         <v>81</v>
@@ -1632,52 +1693,46 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>142</v>
-      </c>
-      <c r="C31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" t="s">
-        <v>83</v>
+        <v>210</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="C33" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1685,27 +1740,27 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>144</v>
+        <v>212</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>217</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1713,27 +1768,33 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C36" t="s">
-        <v>189</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="E36" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>187</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1741,27 +1802,27 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
-        <v>190</v>
+        <v>85</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1769,27 +1830,27 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C41" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1797,27 +1858,27 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C42" t="s">
-        <v>191</v>
+        <v>87</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>189</v>
       </c>
       <c r="D43" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1825,27 +1886,27 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C45" t="s">
-        <v>192</v>
+        <v>89</v>
       </c>
       <c r="D45" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1853,27 +1914,27 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D47" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1881,30 +1942,27 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D48" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" t="s">
-        <v>183</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C49" t="s">
-        <v>95</v>
+        <v>191</v>
       </c>
       <c r="D49" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1912,27 +1970,27 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C50" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D50" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D51" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1940,30 +1998,30 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D52" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>52</v>
-      </c>
       <c r="B53" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C53" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D53" t="s">
-        <v>49</v>
-      </c>
-      <c r="E53" t="s">
-        <v>167</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1971,30 +2029,27 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C54" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D54" t="s">
-        <v>101</v>
-      </c>
-      <c r="E54" t="s">
-        <v>167</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C55" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D55" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2002,27 +2057,30 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C56" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D56" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C57" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D57" t="s">
-        <v>102</v>
+        <v>49</v>
+      </c>
+      <c r="E57" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -2030,33 +2088,30 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C58" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D58" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="E58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D59" t="s">
-        <v>67</v>
-      </c>
-      <c r="E59" t="s">
-        <v>167</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -2064,27 +2119,27 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C60" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D60" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C61" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D61" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -2092,27 +2147,33 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C62" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D62" t="s">
-        <v>36</v>
+        <v>66</v>
+      </c>
+      <c r="E62" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C63" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D63" t="s">
-        <v>37</v>
+        <v>67</v>
+      </c>
+      <c r="E63" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -2120,27 +2181,27 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C64" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D64" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C65" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D65" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2148,26 +2209,82 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>173</v>
+      </c>
+      <c r="C66" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>174</v>
+      </c>
+      <c r="C67" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>175</v>
+      </c>
+      <c r="C68" t="s">
+        <v>113</v>
+      </c>
+      <c r="D68" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>176</v>
+      </c>
+      <c r="C69" t="s">
+        <v>112</v>
+      </c>
+      <c r="D69" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>177</v>
+      </c>
+      <c r="C70" t="s">
+        <v>110</v>
+      </c>
+      <c r="D70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
         <v>178</v>
       </c>
-      <c r="C66" t="s">
-        <v>110</v>
-      </c>
-      <c r="D66" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>179</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="C71" t="s">
         <v>111</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D71" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
separate .common and .company
</commit_message>
<xml_diff>
--- a/data/data_fmt_readme.xlsx
+++ b/data/data_fmt_readme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jupyter연습\factors_affecting_stock_price\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEAE94C-F5D8-4BD6-AD6B-9B52A267C78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AF5429-3810-414F-98AA-A5DEC38393C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34515" yWindow="930" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3975" yWindow="1035" windowWidth="20025" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="항목설명" sheetId="2" r:id="rId1"/>
@@ -662,10 +662,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fed_rate-imp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bok_rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -675,10 +671,6 @@
   </si>
   <si>
     <t>bok_rate_ann</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bok_rate-imp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -995,6 +987,14 @@
   </si>
   <si>
     <t>한국2년만기국채수익률 변동률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fed_rate_imp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bok_rate_imp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1332,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1377,10 +1377,10 @@
         <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1394,7 +1394,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1411,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1428,10 +1428,10 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1523,7 +1523,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
         <v>62</v>
@@ -1537,7 +1537,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s">
         <v>63</v>
@@ -1649,13 +1649,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" t="s">
         <v>216</v>
-      </c>
-      <c r="C20" t="s">
-        <v>217</v>
-      </c>
-      <c r="D20" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1663,13 +1663,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" t="s">
         <v>219</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>221</v>
-      </c>
-      <c r="D21" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1677,13 +1677,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" t="s">
         <v>220</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>222</v>
-      </c>
-      <c r="D22" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1705,13 +1705,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" t="s">
         <v>225</v>
-      </c>
-      <c r="C24" t="s">
-        <v>226</v>
-      </c>
-      <c r="D24" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1719,13 +1719,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1733,13 +1733,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>226</v>
+      </c>
+      <c r="C26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" t="s">
         <v>228</v>
-      </c>
-      <c r="C26" t="s">
-        <v>229</v>
-      </c>
-      <c r="D26" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1747,13 +1747,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D27" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1761,13 +1761,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C28" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1775,13 +1775,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1789,13 +1789,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1803,13 +1803,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>190</v>
+      </c>
+      <c r="C31" t="s">
         <v>192</v>
       </c>
-      <c r="C31" t="s">
-        <v>194</v>
-      </c>
       <c r="D31" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1817,13 +1817,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C32" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D32" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1831,13 +1831,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" t="s">
         <v>193</v>
       </c>
-      <c r="C33" t="s">
-        <v>195</v>
-      </c>
       <c r="D33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1845,13 +1845,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D34" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1915,13 +1915,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1929,13 +1929,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D40" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1943,13 +1943,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1957,13 +1957,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D42" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1994,7 +1994,7 @@
         <v>23</v>
       </c>
       <c r="E44" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -2005,13 +2005,13 @@
         <v>148</v>
       </c>
       <c r="C45" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D45" t="s">
         <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -2050,7 +2050,7 @@
         <v>149</v>
       </c>
       <c r="C48" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D48" t="s">
         <v>21</v>
@@ -2092,7 +2092,7 @@
         <v>150</v>
       </c>
       <c r="C51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D51" t="s">
         <v>28</v>
@@ -2134,7 +2134,7 @@
         <v>151</v>
       </c>
       <c r="C54" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D54" t="s">
         <v>31</v>
@@ -2176,7 +2176,7 @@
         <v>152</v>
       </c>
       <c r="C57" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D57" t="s">
         <v>34</v>
@@ -2224,7 +2224,7 @@
         <v>45</v>
       </c>
       <c r="E60" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -2297,7 +2297,7 @@
         <v>49</v>
       </c>
       <c r="E65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -2305,7 +2305,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>161</v>
+        <v>243</v>
       </c>
       <c r="C66" t="s">
         <v>98</v>
@@ -2314,7 +2314,7 @@
         <v>99</v>
       </c>
       <c r="E66" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -2322,7 +2322,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C67" t="s">
         <v>101</v>
@@ -2336,7 +2336,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C68" t="s">
         <v>102</v>
@@ -2350,7 +2350,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>165</v>
+        <v>244</v>
       </c>
       <c r="C69" t="s">
         <v>103</v>
@@ -2364,7 +2364,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C70" t="s">
         <v>104</v>
@@ -2373,7 +2373,7 @@
         <v>66</v>
       </c>
       <c r="E70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2381,7 +2381,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C71" t="s">
         <v>105</v>
@@ -2390,7 +2390,7 @@
         <v>67</v>
       </c>
       <c r="E71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -2398,7 +2398,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C72" t="s">
         <v>106</v>
@@ -2412,7 +2412,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C73" t="s">
         <v>107</v>
@@ -2426,7 +2426,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C74" t="s">
         <v>113</v>
@@ -2440,7 +2440,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C75" t="s">
         <v>112</v>
@@ -2454,7 +2454,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C76" t="s">
         <v>111</v>
@@ -2468,7 +2468,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C77" t="s">
         <v>110</v>
@@ -2482,7 +2482,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C78" t="s">
         <v>108</v>
@@ -2496,7 +2496,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C79" t="s">
         <v>109</v>

</xml_diff>